<commit_message>
Added general skill rework sheet
</commit_message>
<xml_diff>
--- a/Modding resources/Generals rework/Generals_worksheet.xlsx
+++ b/Modding resources/Generals rework/Generals_worksheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niko\Documents\Paradox Interactive\Hearts of Iron IV\mod\Millennium_Dawn\Modding resources\Generals rework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CB624CA-67B1-4980-BF87-CEBA04C877B9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49D4487A-5A65-4BCB-AAAC-7BF6F3BE5863}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="269">
   <si>
     <t>TAG</t>
   </si>
@@ -832,9 +835,6 @@
   </si>
   <si>
     <t>Done</t>
-  </si>
-  <si>
-    <t>x</t>
   </si>
   <si>
     <t>ID min</t>
@@ -1256,7 +1256,7 @@
   <dimension ref="A2:R253"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P29" sqref="P29"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1328,10 +1328,10 @@
         <v>266</v>
       </c>
       <c r="Q2" t="s">
+        <v>267</v>
+      </c>
+      <c r="R2" t="s">
         <v>268</v>
-      </c>
-      <c r="R2" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -1368,9 +1368,7 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-      <c r="P3" s="1" t="s">
-        <v>267</v>
-      </c>
+      <c r="P3" s="1"/>
       <c r="Q3">
         <v>1</v>
       </c>
@@ -1412,9 +1410,7 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-      <c r="P4" s="1" t="s">
-        <v>267</v>
-      </c>
+      <c r="P4" s="1"/>
       <c r="Q4">
         <v>21</v>
       </c>
@@ -1456,9 +1452,7 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>1</v>
       </c>
-      <c r="P5" s="1" t="s">
-        <v>267</v>
-      </c>
+      <c r="P5" s="1"/>
       <c r="Q5">
         <v>41</v>
       </c>
@@ -1500,9 +1494,7 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>-1</v>
       </c>
-      <c r="P6" s="1" t="s">
-        <v>267</v>
-      </c>
+      <c r="P6" s="1"/>
       <c r="Q6">
         <v>61</v>
       </c>
@@ -1544,9 +1536,7 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>1</v>
       </c>
-      <c r="P7" s="1" t="s">
-        <v>267</v>
-      </c>
+      <c r="P7" s="1"/>
       <c r="Q7">
         <v>81</v>
       </c>
@@ -1588,9 +1578,7 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-      <c r="P8" s="1" t="s">
-        <v>267</v>
-      </c>
+      <c r="P8" s="1"/>
       <c r="Q8">
         <v>101</v>
       </c>
@@ -1632,9 +1620,7 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-      <c r="P9" s="1" t="s">
-        <v>267</v>
-      </c>
+      <c r="P9" s="1"/>
       <c r="Q9">
         <v>121</v>
       </c>
@@ -1679,9 +1665,7 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>1</v>
       </c>
-      <c r="P10" s="1" t="s">
-        <v>267</v>
-      </c>
+      <c r="P10" s="1"/>
       <c r="Q10">
         <v>141</v>
       </c>
@@ -1723,9 +1707,7 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-      <c r="P11" s="1" t="s">
-        <v>267</v>
-      </c>
+      <c r="P11" s="1"/>
       <c r="Q11">
         <v>161</v>
       </c>
@@ -1767,9 +1749,7 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-      <c r="P12" s="1" t="s">
-        <v>267</v>
-      </c>
+      <c r="P12" s="1"/>
       <c r="Q12">
         <v>181</v>
       </c>
@@ -1811,9 +1791,7 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-      <c r="P13" s="1" t="s">
-        <v>267</v>
-      </c>
+      <c r="P13" s="1"/>
       <c r="Q13">
         <v>201</v>
       </c>
@@ -1855,9 +1833,7 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>1</v>
       </c>
-      <c r="P14" s="1" t="s">
-        <v>267</v>
-      </c>
+      <c r="P14" s="1"/>
       <c r="Q14">
         <v>221</v>
       </c>
@@ -1905,9 +1881,7 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-      <c r="P15" s="1" t="s">
-        <v>267</v>
-      </c>
+      <c r="P15" s="1"/>
       <c r="Q15">
         <v>241</v>
       </c>
@@ -1949,9 +1923,7 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-      <c r="P16" s="1" t="s">
-        <v>267</v>
-      </c>
+      <c r="P16" s="1"/>
       <c r="Q16">
         <v>261</v>
       </c>
@@ -1993,9 +1965,7 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>1</v>
       </c>
-      <c r="P17" s="1" t="s">
-        <v>267</v>
-      </c>
+      <c r="P17" s="1"/>
       <c r="Q17">
         <v>281</v>
       </c>
@@ -2037,9 +2007,7 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-      <c r="P18" s="1" t="s">
-        <v>267</v>
-      </c>
+      <c r="P18" s="1"/>
       <c r="Q18">
         <v>301</v>
       </c>
@@ -2081,9 +2049,7 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-      <c r="P19" s="1" t="s">
-        <v>267</v>
-      </c>
+      <c r="P19" s="1"/>
       <c r="Q19">
         <v>321</v>
       </c>
@@ -2125,9 +2091,7 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-      <c r="P20" s="1" t="s">
-        <v>267</v>
-      </c>
+      <c r="P20" s="1"/>
       <c r="Q20">
         <v>341</v>
       </c>
@@ -2169,9 +2133,7 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-      <c r="P21" s="1" t="s">
-        <v>267</v>
-      </c>
+      <c r="P21" s="1"/>
       <c r="Q21">
         <v>361</v>
       </c>
@@ -2213,9 +2175,7 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-      <c r="P22" s="1" t="s">
-        <v>267</v>
-      </c>
+      <c r="P22" s="1"/>
       <c r="Q22">
         <v>381</v>
       </c>
@@ -2263,9 +2223,7 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-      <c r="P23" s="1" t="s">
-        <v>267</v>
-      </c>
+      <c r="P23" s="1"/>
       <c r="Q23">
         <v>401</v>
       </c>
@@ -2307,9 +2265,7 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-      <c r="P24" s="1" t="s">
-        <v>267</v>
-      </c>
+      <c r="P24" s="1"/>
       <c r="Q24">
         <v>421</v>
       </c>
@@ -2351,9 +2307,7 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-      <c r="P25" s="1" t="s">
-        <v>267</v>
-      </c>
+      <c r="P25" s="1"/>
       <c r="Q25">
         <v>441</v>
       </c>
@@ -2395,9 +2349,7 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-      <c r="P26" s="1" t="s">
-        <v>267</v>
-      </c>
+      <c r="P26" s="1"/>
       <c r="Q26">
         <v>461</v>
       </c>
@@ -2439,9 +2391,7 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-      <c r="P27" s="1" t="s">
-        <v>267</v>
-      </c>
+      <c r="P27" s="1"/>
       <c r="Q27">
         <v>481</v>
       </c>
@@ -2483,9 +2433,7 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-      <c r="P28" s="1" t="s">
-        <v>267</v>
-      </c>
+      <c r="P28" s="1"/>
       <c r="Q28">
         <v>501</v>
       </c>

</xml_diff>

<commit_message>
Unit leaders ABK to AGL
</commit_message>
<xml_diff>
--- a/Modding resources/Generals rework/Generals_worksheet.xlsx
+++ b/Modding resources/Generals rework/Generals_worksheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niko\Documents\Paradox Interactive\Hearts of Iron IV\mod\Millennium_Dawn\Modding resources\Generals rework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE49AB47-5D73-4C59-AC54-CE61026D0FB2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C34E2275-B4F3-4766-B173-4D09AD38ABC3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Rework" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="449">
   <si>
     <t>TAG</t>
   </si>
@@ -1799,8 +1799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:R253"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1957,7 +1957,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-      <c r="P4" s="1"/>
+      <c r="P4" s="1" t="s">
+        <v>269</v>
+      </c>
       <c r="Q4">
         <v>21</v>
       </c>
@@ -1999,7 +2001,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>1</v>
       </c>
-      <c r="P5" s="1"/>
+      <c r="P5" s="1" t="s">
+        <v>269</v>
+      </c>
       <c r="Q5">
         <v>41</v>
       </c>
@@ -2041,7 +2045,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>-1</v>
       </c>
-      <c r="P6" s="1"/>
+      <c r="P6" s="1" t="s">
+        <v>269</v>
+      </c>
       <c r="Q6">
         <v>61</v>
       </c>
@@ -2083,7 +2089,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>1</v>
       </c>
-      <c r="P7" s="1"/>
+      <c r="P7" s="1" t="s">
+        <v>269</v>
+      </c>
       <c r="Q7">
         <v>81</v>
       </c>
@@ -2125,7 +2133,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-      <c r="P8" s="1"/>
+      <c r="P8" s="1" t="s">
+        <v>269</v>
+      </c>
       <c r="Q8">
         <v>101</v>
       </c>
@@ -12711,8 +12721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19E469F0-E937-4D3B-84E7-469E4E3F14B8}">
   <dimension ref="A2:Q22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Unit leaders ALA & ALB
</commit_message>
<xml_diff>
--- a/Modding resources/Generals rework/Generals_worksheet.xlsx
+++ b/Modding resources/Generals rework/Generals_worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niko\Documents\Paradox Interactive\Hearts of Iron IV\mod\Millennium_Dawn\Modding resources\Generals rework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C34E2275-B4F3-4766-B173-4D09AD38ABC3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09D03D82-7EC0-47A9-BF82-CDDF80DB90BC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="449">
   <si>
     <t>TAG</t>
   </si>
@@ -1800,7 +1800,7 @@
   <dimension ref="A2:R253"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S9" sqref="S9"/>
+      <selection activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2177,7 +2177,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-      <c r="P9" s="1"/>
+      <c r="P9" s="1" t="s">
+        <v>269</v>
+      </c>
       <c r="Q9">
         <v>121</v>
       </c>
@@ -2222,7 +2224,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>1</v>
       </c>
-      <c r="P10" s="1"/>
+      <c r="P10" s="1" t="s">
+        <v>269</v>
+      </c>
       <c r="Q10">
         <v>141</v>
       </c>
@@ -12722,7 +12726,7 @@
   <dimension ref="A2:Q22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Unit leaders ARG & ARM
</commit_message>
<xml_diff>
--- a/Modding resources/Generals rework/Generals_worksheet.xlsx
+++ b/Modding resources/Generals rework/Generals_worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niko\Documents\Paradox Interactive\Hearts of Iron IV\mod\Millennium_Dawn\Modding resources\Generals rework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{924AF80E-0D4B-4C23-9D52-9438E3FD87A7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45FAEF7A-1694-487D-AE6C-D88DBD9D73FE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="449">
   <si>
     <t>TAG</t>
   </si>
@@ -1276,9 +1276,6 @@
     <t>army_concealment_X</t>
   </si>
   <si>
-    <t>navy_sumbarine_X</t>
-  </si>
-  <si>
     <t>navy_screen_X</t>
   </si>
   <si>
@@ -1382,6 +1379,9 @@
   </si>
   <si>
     <t>air_force_multiplier_X (helicopters)</t>
+  </si>
+  <si>
+    <t>navy_submarine_X</t>
   </si>
 </sst>
 </file>
@@ -1800,7 +1800,7 @@
   <dimension ref="A2:R253"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+      <selection activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2400,7 +2400,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>1</v>
       </c>
-      <c r="P14" s="1"/>
+      <c r="P14" s="1" t="s">
+        <v>269</v>
+      </c>
       <c r="Q14">
         <v>221</v>
       </c>
@@ -2448,7 +2450,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-      <c r="P15" s="1"/>
+      <c r="P15" s="1" t="s">
+        <v>269</v>
+      </c>
       <c r="Q15">
         <v>241</v>
       </c>
@@ -12732,7 +12736,7 @@
   <dimension ref="A2:Q22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12821,7 +12825,7 @@
         <v>399</v>
       </c>
       <c r="G3" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="I3" t="s">
         <v>352</v>
@@ -12839,13 +12843,13 @@
         <v>395</v>
       </c>
       <c r="N3" t="s">
-        <v>413</v>
+        <v>448</v>
       </c>
       <c r="O3" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="Q3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -12868,7 +12872,7 @@
         <v>400</v>
       </c>
       <c r="G4" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="I4" t="s">
         <v>353</v>
@@ -12883,13 +12887,13 @@
         <v>396</v>
       </c>
       <c r="N4" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="O4" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="Q4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -12909,7 +12913,7 @@
         <v>401</v>
       </c>
       <c r="G5" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="I5" t="s">
         <v>354</v>
@@ -12927,13 +12931,13 @@
         <v>397</v>
       </c>
       <c r="N5" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="O5" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="Q5" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -12956,7 +12960,7 @@
         <v>402</v>
       </c>
       <c r="G6" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="I6" t="s">
         <v>355</v>
@@ -12974,13 +12978,13 @@
         <v>398</v>
       </c>
       <c r="N6" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="O6" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="Q6" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -13003,7 +13007,7 @@
         <v>403</v>
       </c>
       <c r="G7" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="I7" t="s">
         <v>356</v>
@@ -13018,13 +13022,13 @@
         <v>378</v>
       </c>
       <c r="N7" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="O7" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="Q7" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -13047,7 +13051,7 @@
         <v>404</v>
       </c>
       <c r="G8" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="I8" t="s">
         <v>357</v>
@@ -13056,10 +13060,10 @@
         <v>379</v>
       </c>
       <c r="N8" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="Q8" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -13082,7 +13086,7 @@
         <v>405</v>
       </c>
       <c r="G9" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="I9" t="s">
         <v>358</v>
@@ -13094,10 +13098,10 @@
         <v>381</v>
       </c>
       <c r="N9" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="Q9" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -13117,7 +13121,7 @@
         <v>406</v>
       </c>
       <c r="G10" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="I10" t="s">
         <v>359</v>
@@ -13129,10 +13133,10 @@
         <v>383</v>
       </c>
       <c r="N10" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="Q10" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
@@ -13155,7 +13159,7 @@
         <v>407</v>
       </c>
       <c r="G11" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="I11" t="s">
         <v>360</v>
@@ -13170,7 +13174,7 @@
         <v>386</v>
       </c>
       <c r="Q11" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
@@ -13190,7 +13194,7 @@
         <v>408</v>
       </c>
       <c r="G12" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="I12" t="s">
         <v>361</v>
@@ -13199,7 +13203,7 @@
         <v>387</v>
       </c>
       <c r="Q12" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -13222,7 +13226,7 @@
         <v>388</v>
       </c>
       <c r="Q13" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
@@ -13251,7 +13255,7 @@
         <v>391</v>
       </c>
       <c r="Q14" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
@@ -13277,7 +13281,7 @@
         <v>393</v>
       </c>
       <c r="Q15" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Unit leaders AUS -> BEL
</commit_message>
<xml_diff>
--- a/Modding resources/Generals rework/Generals_worksheet.xlsx
+++ b/Modding resources/Generals rework/Generals_worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niko\Documents\Paradox Interactive\Hearts of Iron IV\mod\Millennium_Dawn\Modding resources\Generals rework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E3F7806-DD9E-4382-839C-0080AC4F8D9E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{403586D6-CC84-4321-BBAE-9C898E8AA8B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="449">
   <si>
     <t>TAG</t>
   </si>
@@ -1437,9 +1437,6 @@
   </cellStyles>
   <dxfs count="5">
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <color auto="1"/>
       </font>
@@ -1478,6 +1475,9 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1526,7 +1526,7 @@
     <tableColumn id="15" xr3:uid="{AD6381E7-3290-44E4-9E98-E7E9063F54F9}" name="DeltaFM">
       <calculatedColumnFormula>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{F1A1B7D8-F172-48DC-AF4F-5C441C6D421B}" name="Done" dataDxfId="0"/>
+    <tableColumn id="16" xr3:uid="{F1A1B7D8-F172-48DC-AF4F-5C441C6D421B}" name="Done" dataDxfId="4"/>
     <tableColumn id="17" xr3:uid="{C49D052D-3754-49A2-9551-F2176AA27932}" name="ID min"/>
     <tableColumn id="18" xr3:uid="{8A6F4AEA-EC4E-4C6E-A653-1A392AFA8658}" name="ID max"/>
   </tableColumns>
@@ -1799,8 +1799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:R253"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="P24" sqref="P24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2538,7 +2538,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>1</v>
       </c>
-      <c r="P17" s="1"/>
+      <c r="P17" s="1" t="s">
+        <v>269</v>
+      </c>
       <c r="Q17">
         <v>281</v>
       </c>
@@ -2580,7 +2582,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-      <c r="P18" s="1"/>
+      <c r="P18" s="1" t="s">
+        <v>269</v>
+      </c>
       <c r="Q18">
         <v>301</v>
       </c>
@@ -2622,7 +2626,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-      <c r="P19" s="1"/>
+      <c r="P19" s="1" t="s">
+        <v>269</v>
+      </c>
       <c r="Q19">
         <v>321</v>
       </c>
@@ -2664,7 +2670,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-      <c r="P20" s="1"/>
+      <c r="P20" s="1" t="s">
+        <v>269</v>
+      </c>
       <c r="Q20">
         <v>341</v>
       </c>
@@ -2706,7 +2714,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-      <c r="P21" s="1"/>
+      <c r="P21" s="1" t="s">
+        <v>269</v>
+      </c>
       <c r="Q21">
         <v>361</v>
       </c>
@@ -2748,7 +2758,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-      <c r="P22" s="1"/>
+      <c r="P22" s="1" t="s">
+        <v>269</v>
+      </c>
       <c r="Q22">
         <v>381</v>
       </c>
@@ -2796,7 +2808,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-      <c r="P23" s="1"/>
+      <c r="P23" s="1" t="s">
+        <v>269</v>
+      </c>
       <c r="Q23">
         <v>401</v>
       </c>
@@ -12710,18 +12724,18 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="N3:O253">
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P3:P253">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12738,7 +12752,7 @@
   <dimension ref="A2:Q22"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Unit leaders BEN -> BHR
</commit_message>
<xml_diff>
--- a/Modding resources/Generals rework/Generals_worksheet.xlsx
+++ b/Modding resources/Generals rework/Generals_worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niko\Documents\Paradox Interactive\Hearts of Iron IV\mod\Millennium_Dawn\Modding resources\Generals rework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{403586D6-CC84-4321-BBAE-9C898E8AA8B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6713A43B-57E8-4D66-83F8-2CFE4AA24074}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="449">
   <si>
     <t>TAG</t>
   </si>
@@ -1437,6 +1437,9 @@
   </cellStyles>
   <dxfs count="5">
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <color auto="1"/>
       </font>
@@ -1475,9 +1478,6 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1526,7 +1526,7 @@
     <tableColumn id="15" xr3:uid="{AD6381E7-3290-44E4-9E98-E7E9063F54F9}" name="DeltaFM">
       <calculatedColumnFormula>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{F1A1B7D8-F172-48DC-AF4F-5C441C6D421B}" name="Done" dataDxfId="4"/>
+    <tableColumn id="16" xr3:uid="{F1A1B7D8-F172-48DC-AF4F-5C441C6D421B}" name="Done" dataDxfId="0"/>
     <tableColumn id="17" xr3:uid="{C49D052D-3754-49A2-9551-F2176AA27932}" name="ID min"/>
     <tableColumn id="18" xr3:uid="{8A6F4AEA-EC4E-4C6E-A653-1A392AFA8658}" name="ID max"/>
   </tableColumns>
@@ -1800,7 +1800,7 @@
   <dimension ref="A2:R253"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="P24" sqref="P24"/>
+      <selection activeCell="P27" sqref="P27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2852,7 +2852,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-      <c r="P24" s="1"/>
+      <c r="P24" s="1" t="s">
+        <v>269</v>
+      </c>
       <c r="Q24">
         <v>421</v>
       </c>
@@ -2894,7 +2896,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-      <c r="P25" s="1"/>
+      <c r="P25" s="1" t="s">
+        <v>269</v>
+      </c>
       <c r="Q25">
         <v>441</v>
       </c>
@@ -2936,7 +2940,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-      <c r="P26" s="1"/>
+      <c r="P26" s="1" t="s">
+        <v>269</v>
+      </c>
       <c r="Q26">
         <v>461</v>
       </c>
@@ -12724,18 +12730,18 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="N3:O253">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P3:P253">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12752,7 +12758,7 @@
   <dimension ref="A2:Q22"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
BHU & BLC unit leaders
</commit_message>
<xml_diff>
--- a/Modding resources/Generals rework/Generals_worksheet.xlsx
+++ b/Modding resources/Generals rework/Generals_worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niko\Documents\Paradox Interactive\Hearts of Iron IV\mod\Millennium_Dawn\Modding resources\Generals rework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6713A43B-57E8-4D66-83F8-2CFE4AA24074}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD93565A-1C75-41FD-A4AA-71E0E9AC30E4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="449">
   <si>
     <t>TAG</t>
   </si>
@@ -1800,7 +1800,7 @@
   <dimension ref="A2:R253"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="P27" sqref="P27"/>
+      <selection activeCell="P29" sqref="P29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2984,7 +2984,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-      <c r="P27" s="1"/>
+      <c r="P27" s="1" t="s">
+        <v>269</v>
+      </c>
       <c r="Q27">
         <v>481</v>
       </c>
@@ -3026,7 +3028,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-      <c r="P28" s="1"/>
+      <c r="P28" s="1" t="s">
+        <v>269</v>
+      </c>
       <c r="Q28">
         <v>501</v>
       </c>
@@ -12757,8 +12761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19E469F0-E937-4D3B-84E7-469E4E3F14B8}">
   <dimension ref="A2:Q22"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Unit leaders BLR & BLZ
</commit_message>
<xml_diff>
--- a/Modding resources/Generals rework/Generals_worksheet.xlsx
+++ b/Modding resources/Generals rework/Generals_worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niko\Documents\Paradox Interactive\Hearts of Iron IV\mod\Millennium_Dawn\Modding resources\Generals rework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD93565A-1C75-41FD-A4AA-71E0E9AC30E4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46606D74-BCA6-47C7-95C1-EB4695EECA08}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="449">
   <si>
     <t>TAG</t>
   </si>
@@ -1800,7 +1800,7 @@
   <dimension ref="A2:R253"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="P29" sqref="P29"/>
+      <selection activeCell="P31" sqref="P31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3078,7 +3078,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-      <c r="P29" s="1"/>
+      <c r="P29" s="1" t="s">
+        <v>269</v>
+      </c>
       <c r="Q29">
         <v>521</v>
       </c>
@@ -3120,7 +3122,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-      <c r="P30" s="1"/>
+      <c r="P30" s="1" t="s">
+        <v>269</v>
+      </c>
       <c r="Q30">
         <v>541</v>
       </c>
@@ -12761,8 +12765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19E469F0-E937-4D3B-84E7-469E4E3F14B8}">
   <dimension ref="A2:Q22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
DAR -> DRU unit leaders
</commit_message>
<xml_diff>
--- a/Modding resources/Generals rework/Generals_worksheet.xlsx
+++ b/Modding resources/Generals rework/Generals_worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niko\Documents\Paradox Interactive\Hearts of Iron IV\mod\Millennium_Dawn\Modding resources\Generals rework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{605A20FD-FFD1-4DA0-978E-365F7597D140}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E72A2C83-3929-43F4-A682-1361FE198C53}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="451">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="451">
   <si>
     <t>TAG</t>
   </si>
@@ -1443,9 +1443,6 @@
   </cellStyles>
   <dxfs count="5">
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <color auto="1"/>
       </font>
@@ -1484,6 +1481,9 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1532,7 +1532,7 @@
     <tableColumn id="15" xr3:uid="{AD6381E7-3290-44E4-9E98-E7E9063F54F9}" name="DeltaFM">
       <calculatedColumnFormula>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{F1A1B7D8-F172-48DC-AF4F-5C441C6D421B}" name="Done" dataDxfId="0"/>
+    <tableColumn id="16" xr3:uid="{F1A1B7D8-F172-48DC-AF4F-5C441C6D421B}" name="Done" dataDxfId="4"/>
     <tableColumn id="17" xr3:uid="{C49D052D-3754-49A2-9551-F2176AA27932}" name="ID min"/>
     <tableColumn id="18" xr3:uid="{8A6F4AEA-EC4E-4C6E-A653-1A392AFA8658}" name="ID max"/>
   </tableColumns>
@@ -1805,8 +1805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:R255"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="P62" sqref="P62"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="P69" sqref="P69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4542,7 +4542,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-      <c r="P62" s="1"/>
+      <c r="P62" s="1" t="s">
+        <v>269</v>
+      </c>
       <c r="Q62">
         <v>1141</v>
       </c>
@@ -4634,7 +4636,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-      <c r="P64" s="1"/>
+      <c r="P64" s="1" t="s">
+        <v>269</v>
+      </c>
       <c r="Q64">
         <v>1181</v>
       </c>
@@ -4676,7 +4680,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-      <c r="P65" s="1"/>
+      <c r="P65" s="1" t="s">
+        <v>269</v>
+      </c>
       <c r="Q65">
         <v>1201</v>
       </c>
@@ -4718,7 +4724,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-      <c r="P66" s="1"/>
+      <c r="P66" s="1" t="s">
+        <v>269</v>
+      </c>
       <c r="Q66">
         <v>1221</v>
       </c>
@@ -4760,7 +4768,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-      <c r="P67" s="1"/>
+      <c r="P67" s="1" t="s">
+        <v>269</v>
+      </c>
       <c r="Q67">
         <v>1241</v>
       </c>
@@ -4802,7 +4812,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-      <c r="P68" s="1"/>
+      <c r="P68" s="1" t="s">
+        <v>269</v>
+      </c>
       <c r="Q68">
         <v>1261</v>
       </c>
@@ -12876,18 +12888,18 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="N3:O255">
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P3:P255">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12904,7 +12916,7 @@
   <dimension ref="A2:Q22"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Officer rework done for Macedonia. Also some corrections of some generals skills.
</commit_message>
<xml_diff>
--- a/Modding resources/Generals rework/Generals_worksheet.xlsx
+++ b/Modding resources/Generals rework/Generals_worksheet.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niko\Documents\Paradox Interactive\Hearts of Iron IV\mod\Millennium_Dawn\Modding resources\Generals rework\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Misagh.H\Documents\Paradox Interactive\Hearts of Iron IV\mod\Millennium_Dawn\Millennium_Dawn_DEV\Modding resources\Generals rework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78B5B0B1-CE85-4FAB-B1F8-E105E8D112CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="General Rework" sheetId="1" r:id="rId1"/>
     <sheet name="Trait List" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="452">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="452">
   <si>
     <t>TAG</t>
   </si>
@@ -1396,7 +1395,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1442,7 +1441,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normaali" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="5">
     <dxf>
@@ -1502,42 +1501,42 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{10BD23E6-60AB-42C7-B043-A8B30FF8C033}" name="Taulukko2" displayName="Taulukko2" ref="A2:R256" totalsRowShown="0">
-  <autoFilter ref="A2:R256" xr:uid="{6DDEF623-4240-4F7B-A4DC-C137388F3BBA}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:O256">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Taulukko2" displayName="Taulukko2" ref="A2:R256" totalsRowShown="0">
+  <autoFilter ref="A2:R256"/>
+  <sortState ref="A3:O256">
     <sortCondition ref="A2:A256"/>
   </sortState>
   <tableColumns count="18">
-    <tableColumn id="1" xr3:uid="{0F370F1D-33D6-4690-B3B1-6018D18D0D34}" name="TAG"/>
-    <tableColumn id="2" xr3:uid="{A251529F-C198-4882-980D-186989E9B99C}" name="Units 1"/>
-    <tableColumn id="3" xr3:uid="{7E1D6517-8E7B-4427-B6C9-14389192DE8B}" name="Is Major 1"/>
-    <tableColumn id="4" xr3:uid="{588C3809-C9CA-4AEA-9EF0-533C64E739E4}" name="Is in Faction 1"/>
-    <tableColumn id="5" xr3:uid="{BCCB4B03-5F7F-44EB-9901-B606126976C3}" name="Is Nato 1"/>
-    <tableColumn id="6" xr3:uid="{44BAFD9D-822B-4663-B280-3DE4FEA8BB69}" name="No of Gens 1">
+    <tableColumn id="1" name="TAG"/>
+    <tableColumn id="2" name="Units 1"/>
+    <tableColumn id="3" name="Is Major 1"/>
+    <tableColumn id="4" name="Is in Faction 1"/>
+    <tableColumn id="5" name="Is Nato 1"/>
+    <tableColumn id="6" name="No of Gens 1">
       <calculatedColumnFormula>ROUND(Taulukko2[[#This Row],[Units 1]]/15,0)+1+Taulukko2[[#This Row],[Is Major 1]]+Taulukko2[[#This Row],[Is in Faction 1]]+Taulukko2[[#This Row],[Is Nato 1]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{197C5B3F-B43B-4A81-ACD0-74C7949DAA61}" name="No of FMs 1">
+    <tableColumn id="7" name="No of FMs 1">
       <calculatedColumnFormula>ROUND(Taulukko2[[#This Row],[No of Gens 1]]/3,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{FF51BC1D-EA0A-40F6-9D8C-3D1FE4BCF8C4}" name="Units 2"/>
-    <tableColumn id="9" xr3:uid="{49589B77-E62E-4D08-96EA-7877AEB0D0EE}" name="Is Major 2"/>
-    <tableColumn id="10" xr3:uid="{586137D4-3C4D-4543-9BFB-6E492F8AA6CF}" name="Is in Faction 2"/>
-    <tableColumn id="11" xr3:uid="{0C7687F4-429E-4266-936C-B122FB9E9DC6}" name="Is Nato 2"/>
-    <tableColumn id="12" xr3:uid="{BB7F4C2D-E9D6-4786-A46D-3B04A81F33AB}" name="No of Gens 2">
+    <tableColumn id="8" name="Units 2"/>
+    <tableColumn id="9" name="Is Major 2"/>
+    <tableColumn id="10" name="Is in Faction 2"/>
+    <tableColumn id="11" name="Is Nato 2"/>
+    <tableColumn id="12" name="No of Gens 2">
       <calculatedColumnFormula>ROUND(Taulukko2[[#This Row],[Units 2]]/15,0)+1+Taulukko2[[#This Row],[Is Major 2]]+Taulukko2[[#This Row],[Is in Faction 2]]+Taulukko2[[#This Row],[Is Nato 2]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{BB43CEF2-1EEA-4030-8A67-A9CA835A06EA}" name="No of FMs 2">
+    <tableColumn id="13" name="No of FMs 2">
       <calculatedColumnFormula>ROUND(Taulukko2[[#This Row],[No of Gens 2]]/3,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{68AAE598-9B8F-45FA-A989-9EEA87297881}" name="DeltaG">
+    <tableColumn id="14" name="DeltaG">
       <calculatedColumnFormula>Taulukko2[[#This Row],[No of Gens 2]]-Taulukko2[[#This Row],[No of Gens 1]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{AD6381E7-3290-44E4-9E98-E7E9063F54F9}" name="DeltaFM">
+    <tableColumn id="15" name="DeltaFM">
       <calculatedColumnFormula>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{F1A1B7D8-F172-48DC-AF4F-5C441C6D421B}" name="Done" dataDxfId="0"/>
-    <tableColumn id="17" xr3:uid="{C49D052D-3754-49A2-9551-F2176AA27932}" name="ID min"/>
-    <tableColumn id="18" xr3:uid="{8A6F4AEA-EC4E-4C6E-A653-1A392AFA8658}" name="ID max"/>
+    <tableColumn id="16" name="Done" dataDxfId="0"/>
+    <tableColumn id="17" name="ID min"/>
+    <tableColumn id="18" name="ID max"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1805,11 +1804,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:R256"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="P78" sqref="P78"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H82" sqref="H82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5433,7 +5432,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-      <c r="P82" s="1"/>
+      <c r="P82" s="1" t="s">
+        <v>269</v>
+      </c>
       <c r="Q82">
         <v>1521</v>
       </c>
@@ -12981,7 +12982,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19E469F0-E937-4D3B-84E7-469E4E3F14B8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Q22"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">

</xml_diff>

<commit_message>
Iranian Generals for 2000 and 2017 is done.
</commit_message>
<xml_diff>
--- a/Modding resources/Generals rework/Generals_worksheet.xlsx
+++ b/Modding resources/Generals rework/Generals_worksheet.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="452">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="452">
   <si>
     <t>TAG</t>
   </si>
@@ -1807,8 +1807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:R256"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H82" sqref="H82"/>
+    <sheetView tabSelected="1" topLeftCell="B234" workbookViewId="0">
+      <selection activeCell="F148" sqref="F148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9403,7 +9403,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>1</v>
       </c>
-      <c r="P174" s="1"/>
+      <c r="P174" s="1" t="s">
+        <v>269</v>
+      </c>
       <c r="Q174">
         <v>3361</v>
       </c>

</xml_diff>

<commit_message>
Kuwait generals done. UAE generals done. Iraq 2017 & Syria 2000 generals also done.
</commit_message>
<xml_diff>
--- a/Modding resources/Generals rework/Generals_worksheet.xlsx
+++ b/Modding resources/Generals rework/Generals_worksheet.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="452">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="452">
   <si>
     <t>TAG</t>
   </si>
@@ -1807,8 +1807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:R256"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B234" workbookViewId="0">
-      <selection activeCell="F148" sqref="F148"/>
+    <sheetView tabSelected="1" topLeftCell="B218" workbookViewId="0">
+      <selection activeCell="S228" sqref="S228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6657,7 +6657,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-      <c r="P110" s="1"/>
+      <c r="P110" s="1" t="s">
+        <v>269</v>
+      </c>
       <c r="Q110">
         <v>2081</v>
       </c>
@@ -7307,7 +7309,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-      <c r="P125" s="1"/>
+      <c r="P125" s="1" t="s">
+        <v>269</v>
+      </c>
       <c r="Q125">
         <v>2381</v>
       </c>
@@ -11729,7 +11733,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-      <c r="P228" s="1"/>
+      <c r="P228" s="1" t="s">
+        <v>269</v>
+      </c>
       <c r="Q228">
         <v>4441</v>
       </c>
@@ -12377,7 +12383,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-      <c r="P243" s="1"/>
+      <c r="P243" s="1" t="s">
+        <v>269</v>
+      </c>
       <c r="Q243">
         <v>4741</v>
       </c>

</xml_diff>

<commit_message>
Correcting the generals entry lines in country/history files. + Saudi generals are done.
</commit_message>
<xml_diff>
--- a/Modding resources/Generals rework/Generals_worksheet.xlsx
+++ b/Modding resources/Generals rework/Generals_worksheet.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="452">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="452">
   <si>
     <t>TAG</t>
   </si>
@@ -1807,8 +1807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:R256"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B218" workbookViewId="0">
-      <selection activeCell="S228" sqref="S228"/>
+    <sheetView tabSelected="1" topLeftCell="C211" workbookViewId="0">
+      <selection activeCell="S193" sqref="S193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10237,7 +10237,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>1</v>
       </c>
-      <c r="P193" s="1"/>
+      <c r="P193" s="1" t="s">
+        <v>269</v>
+      </c>
       <c r="Q193">
         <v>3741</v>
       </c>

</xml_diff>

<commit_message>
Generals rework for Jordan, Oman and Qatar.
</commit_message>
<xml_diff>
--- a/Modding resources/Generals rework/Generals_worksheet.xlsx
+++ b/Modding resources/Generals rework/Generals_worksheet.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="452">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="452">
   <si>
     <t>TAG</t>
   </si>
@@ -1807,8 +1807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:R256"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C211" workbookViewId="0">
-      <selection activeCell="S193" sqref="S193"/>
+    <sheetView tabSelected="1" topLeftCell="B160" workbookViewId="0">
+      <selection activeCell="S167" sqref="S167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6923,7 +6923,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-      <c r="P116" s="1"/>
+      <c r="P116" s="1" t="s">
+        <v>269</v>
+      </c>
       <c r="Q116">
         <v>2201</v>
       </c>
@@ -9107,7 +9109,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>1</v>
       </c>
-      <c r="P167" s="1"/>
+      <c r="P167" s="1" t="s">
+        <v>269</v>
+      </c>
       <c r="Q167">
         <v>3221</v>
       </c>
@@ -9799,7 +9803,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-      <c r="P183" s="1"/>
+      <c r="P183" s="1" t="s">
+        <v>269</v>
+      </c>
       <c r="Q183">
         <v>3541</v>
       </c>

</xml_diff>

<commit_message>
TIB, TIM, TNZ, TOG, TRI Characters
</commit_message>
<xml_diff>
--- a/Modding resources/Generals rework/Generals_worksheet.xlsx
+++ b/Modding resources/Generals rework/Generals_worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\levia\OneDrive\Dokumente\Paradox Interactive\Hearts of Iron IV\mod\Millennium_Dawn\Modding resources\Generals rework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD5330E-E788-47C7-BC5E-D230CB6DB55B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{207ED174-B0AA-4937-8E8A-02B89EBA40FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="454">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="454">
   <si>
     <t>TAG</t>
   </si>
@@ -1814,8 +1814,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:R258"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A217" workbookViewId="0">
-      <selection activeCell="S238" sqref="S238"/>
+    <sheetView tabSelected="1" topLeftCell="A203" workbookViewId="0">
+      <selection activeCell="P219" sqref="P219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12108,7 +12108,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-      <c r="P235" s="1"/>
+      <c r="P235" s="1" t="s">
+        <v>269</v>
+      </c>
       <c r="Q235">
         <v>4541</v>
       </c>
@@ -12150,7 +12152,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-      <c r="P236" s="1"/>
+      <c r="P236" s="1" t="s">
+        <v>269</v>
+      </c>
       <c r="Q236">
         <v>4561</v>
       </c>
@@ -12192,7 +12196,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-      <c r="P237" s="1"/>
+      <c r="P237" s="1" t="s">
+        <v>269</v>
+      </c>
       <c r="Q237">
         <v>4581</v>
       </c>
@@ -12234,7 +12240,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-      <c r="P238" s="1"/>
+      <c r="P238" s="1" t="s">
+        <v>269</v>
+      </c>
       <c r="Q238">
         <v>4601</v>
       </c>
@@ -12276,7 +12284,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>0</v>
       </c>
-      <c r="P239" s="1"/>
+      <c r="P239" s="1" t="s">
+        <v>269</v>
+      </c>
       <c r="Q239">
         <v>4621</v>
       </c>

</xml_diff>

<commit_message>
Reworked GRE officer corps
</commit_message>
<xml_diff>
--- a/Modding resources/Generals rework/Generals_worksheet.xlsx
+++ b/Modding resources/Generals rework/Generals_worksheet.xlsx
@@ -1,26 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Misagh.H\Documents\Paradox Interactive\Hearts of Iron IV\mod\Millennium_Dawn\Millennium_Dawn_DEV\Modding resources\Generals rework\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niko\Documents\Paradox Interactive\Hearts of Iron IV\mod\Millennium_Dawn\Modding resources\Generals rework\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{876B8263-9597-4A8C-9A04-EB7DEE7B522C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Rework" sheetId="1" r:id="rId1"/>
     <sheet name="Trait List" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -1404,7 +1408,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1446,7 +1450,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normaali" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
     <dxf>
@@ -1571,27 +1575,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Taulukko2" displayName="Taulukko2" ref="A2:R260" totalsRowShown="0">
-  <autoFilter ref="A2:R260"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Taulukko2" displayName="Taulukko2" ref="A2:R260" totalsRowShown="0">
+  <autoFilter ref="A2:R260" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="18">
-    <tableColumn id="1" name="TAG"/>
-    <tableColumn id="2" name="Units 1"/>
-    <tableColumn id="3" name="Is Major 1"/>
-    <tableColumn id="4" name="Is in Faction 1"/>
-    <tableColumn id="5" name="Is Nato 1"/>
-    <tableColumn id="6" name="No of Gens 1"/>
-    <tableColumn id="7" name="No of FMs 1"/>
-    <tableColumn id="8" name="Units 2"/>
-    <tableColumn id="9" name="Is Major 2"/>
-    <tableColumn id="10" name="Is in Faction 2"/>
-    <tableColumn id="11" name="Is Nato 2"/>
-    <tableColumn id="12" name="No of Gens 2"/>
-    <tableColumn id="13" name="No of FMs 2"/>
-    <tableColumn id="14" name="DeltaG"/>
-    <tableColumn id="15" name="DeltaFM"/>
-    <tableColumn id="16" name="Done"/>
-    <tableColumn id="17" name="ID min"/>
-    <tableColumn id="18" name="ID max"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="TAG"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Units 1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Is Major 1"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Is in Faction 1"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Is Nato 1"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="No of Gens 1"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="No of FMs 1"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Units 2"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Is Major 2"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Is in Faction 2"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Is Nato 2"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="No of Gens 2"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="No of FMs 2"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="DeltaG"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="DeltaFM"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Done"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="ID min"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="ID max"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1893,11 +1897,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:R260"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B212" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D218" sqref="D218"/>
+    <sheetView tabSelected="1" topLeftCell="A81" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P93" sqref="P93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13386,11 +13390,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:Q22"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
rest of SLO generals/advisors
</commit_message>
<xml_diff>
--- a/Modding resources/Generals rework/Generals_worksheet.xlsx
+++ b/Modding resources/Generals rework/Generals_worksheet.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Misagh.H\Documents\Paradox Interactive\Hearts of Iron IV\mod\Millennium_Dawn\Millennium_Dawn_DEV\Modding resources\Generals rework\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jakub\Documents\Paradox Interactive\Hearts of Iron IV\mod\Millennium_Dawn\Modding resources\Generals rework\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC48B88D-898C-4D18-AA41-9E14855C0B57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Rework" sheetId="1" r:id="rId1"/>
     <sheet name="Trait List" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -24,6 +25,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="467">
   <si>
     <t>TAG</t>
   </si>
@@ -1440,7 +1442,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1482,7 +1484,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
     <dxf>
@@ -1607,27 +1609,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Taulukko2" displayName="Taulukko2" ref="A2:R271" totalsRowShown="0">
-  <autoFilter ref="A2:R271"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Taulukko2" displayName="Taulukko2" ref="A2:R271" totalsRowShown="0">
+  <autoFilter ref="A2:R271" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="18">
-    <tableColumn id="1" name="TAG"/>
-    <tableColumn id="2" name="Units 1"/>
-    <tableColumn id="3" name="Is Major 1"/>
-    <tableColumn id="4" name="Is in Faction 1"/>
-    <tableColumn id="5" name="Is Nato 1"/>
-    <tableColumn id="6" name="No of Gens 1"/>
-    <tableColumn id="7" name="No of FMs 1"/>
-    <tableColumn id="8" name="Units 2"/>
-    <tableColumn id="9" name="Is Major 2"/>
-    <tableColumn id="10" name="Is in Faction 2"/>
-    <tableColumn id="11" name="Is Nato 2"/>
-    <tableColumn id="12" name="No of Gens 2"/>
-    <tableColumn id="13" name="No of FMs 2"/>
-    <tableColumn id="14" name="DeltaG"/>
-    <tableColumn id="15" name="DeltaFM"/>
-    <tableColumn id="16" name="Done"/>
-    <tableColumn id="17" name="ID min"/>
-    <tableColumn id="18" name="ID max"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="TAG"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Units 1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Is Major 1"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Is in Faction 1"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Is Nato 1"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="No of Gens 1"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="No of FMs 1"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Units 2"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Is Major 2"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Is in Faction 2"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Is Nato 2"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="No of Gens 2"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="No of FMs 2"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="DeltaG"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="DeltaFM"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Done"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="ID min"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="ID max"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1929,11 +1931,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:R271"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B214" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L225" sqref="L225"/>
+    <sheetView tabSelected="1" topLeftCell="A132" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J147" sqref="J147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11189,7 +11191,7 @@
         <v>225</v>
       </c>
       <c r="B214">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F214">
         <f>ROUND(Taulukko2[[#This Row],[Units 1]]/15,0)+1+Taulukko2[[#This Row],[Is Major 1]]+Taulukko2[[#This Row],[Is in Faction 1]]+Taulukko2[[#This Row],[Is Nato 1]]</f>
@@ -11221,7 +11223,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>1</v>
       </c>
-      <c r="P214" s="3"/>
+      <c r="P214" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="Q214">
         <v>4001</v>
       </c>
@@ -13538,7 +13542,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:Q22"/>
   <sheetViews>
     <sheetView topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">

</xml_diff>

<commit_message>
Revert "Merge branch 'bug-fixes' of https://gitlab.com/Millennium_Dawn/Millennium_Dawn into bug-fixes"
This reverts commit c3c403383f02ddc7c3539583e93e6c7f67a8ce86, reversing
changes made to 902271dbc95bdda59294b8daa401646732208b08.
</commit_message>
<xml_diff>
--- a/Modding resources/Generals rework/Generals_worksheet.xlsx
+++ b/Modding resources/Generals rework/Generals_worksheet.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jakub\Documents\Paradox Interactive\Hearts of Iron IV\mod\Millennium_Dawn\Modding resources\Generals rework\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Misagh.H\Documents\Paradox Interactive\Hearts of Iron IV\mod\Millennium_Dawn\Millennium_Dawn_DEV\Modding resources\Generals rework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC48B88D-898C-4D18-AA41-9E14855C0B57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="General Rework" sheetId="1" r:id="rId1"/>
     <sheet name="Trait List" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -25,7 +24,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="467">
   <si>
     <t>TAG</t>
   </si>
@@ -1442,7 +1440,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1484,7 +1482,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normální" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
     <dxf>
@@ -1609,27 +1607,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Taulukko2" displayName="Taulukko2" ref="A2:R271" totalsRowShown="0">
-  <autoFilter ref="A2:R271" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Taulukko2" displayName="Taulukko2" ref="A2:R271" totalsRowShown="0">
+  <autoFilter ref="A2:R271"/>
   <tableColumns count="18">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="TAG"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Units 1"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Is Major 1"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Is in Faction 1"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Is Nato 1"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="No of Gens 1"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="No of FMs 1"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Units 2"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Is Major 2"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Is in Faction 2"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Is Nato 2"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="No of Gens 2"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="No of FMs 2"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="DeltaG"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="DeltaFM"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Done"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="ID min"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="ID max"/>
+    <tableColumn id="1" name="TAG"/>
+    <tableColumn id="2" name="Units 1"/>
+    <tableColumn id="3" name="Is Major 1"/>
+    <tableColumn id="4" name="Is in Faction 1"/>
+    <tableColumn id="5" name="Is Nato 1"/>
+    <tableColumn id="6" name="No of Gens 1"/>
+    <tableColumn id="7" name="No of FMs 1"/>
+    <tableColumn id="8" name="Units 2"/>
+    <tableColumn id="9" name="Is Major 2"/>
+    <tableColumn id="10" name="Is in Faction 2"/>
+    <tableColumn id="11" name="Is Nato 2"/>
+    <tableColumn id="12" name="No of Gens 2"/>
+    <tableColumn id="13" name="No of FMs 2"/>
+    <tableColumn id="14" name="DeltaG"/>
+    <tableColumn id="15" name="DeltaFM"/>
+    <tableColumn id="16" name="Done"/>
+    <tableColumn id="17" name="ID min"/>
+    <tableColumn id="18" name="ID max"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1931,11 +1929,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:R271"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A132" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J147" sqref="J147"/>
+    <sheetView tabSelected="1" topLeftCell="B214" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L225" sqref="L225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11191,7 +11189,7 @@
         <v>225</v>
       </c>
       <c r="B214">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F214">
         <f>ROUND(Taulukko2[[#This Row],[Units 1]]/15,0)+1+Taulukko2[[#This Row],[Is Major 1]]+Taulukko2[[#This Row],[Is in Faction 1]]+Taulukko2[[#This Row],[Is Nato 1]]</f>
@@ -11223,9 +11221,7 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>1</v>
       </c>
-      <c r="P214" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="P214" s="3"/>
       <c r="Q214">
         <v>4001</v>
       </c>
@@ -13542,7 +13538,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Q22"/>
   <sheetViews>
     <sheetView topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">

</xml_diff>

<commit_message>
Revert "Revert "Merge branch 'bug-fixes' of https://gitlab.com/Millennium_Dawn/Millennium_Dawn into bug-fixes""
This reverts commit 6fb07d383e366330664f047a785845e54210b3e1.
</commit_message>
<xml_diff>
--- a/Modding resources/Generals rework/Generals_worksheet.xlsx
+++ b/Modding resources/Generals rework/Generals_worksheet.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Misagh.H\Documents\Paradox Interactive\Hearts of Iron IV\mod\Millennium_Dawn\Millennium_Dawn_DEV\Modding resources\Generals rework\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jakub\Documents\Paradox Interactive\Hearts of Iron IV\mod\Millennium_Dawn\Modding resources\Generals rework\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC48B88D-898C-4D18-AA41-9E14855C0B57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Rework" sheetId="1" r:id="rId1"/>
     <sheet name="Trait List" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -24,6 +25,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="467">
   <si>
     <t>TAG</t>
   </si>
@@ -1440,7 +1442,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1482,7 +1484,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
     <dxf>
@@ -1607,27 +1609,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Taulukko2" displayName="Taulukko2" ref="A2:R271" totalsRowShown="0">
-  <autoFilter ref="A2:R271"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Taulukko2" displayName="Taulukko2" ref="A2:R271" totalsRowShown="0">
+  <autoFilter ref="A2:R271" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="18">
-    <tableColumn id="1" name="TAG"/>
-    <tableColumn id="2" name="Units 1"/>
-    <tableColumn id="3" name="Is Major 1"/>
-    <tableColumn id="4" name="Is in Faction 1"/>
-    <tableColumn id="5" name="Is Nato 1"/>
-    <tableColumn id="6" name="No of Gens 1"/>
-    <tableColumn id="7" name="No of FMs 1"/>
-    <tableColumn id="8" name="Units 2"/>
-    <tableColumn id="9" name="Is Major 2"/>
-    <tableColumn id="10" name="Is in Faction 2"/>
-    <tableColumn id="11" name="Is Nato 2"/>
-    <tableColumn id="12" name="No of Gens 2"/>
-    <tableColumn id="13" name="No of FMs 2"/>
-    <tableColumn id="14" name="DeltaG"/>
-    <tableColumn id="15" name="DeltaFM"/>
-    <tableColumn id="16" name="Done"/>
-    <tableColumn id="17" name="ID min"/>
-    <tableColumn id="18" name="ID max"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="TAG"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Units 1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Is Major 1"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Is in Faction 1"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Is Nato 1"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="No of Gens 1"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="No of FMs 1"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Units 2"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Is Major 2"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Is in Faction 2"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Is Nato 2"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="No of Gens 2"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="No of FMs 2"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="DeltaG"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="DeltaFM"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Done"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="ID min"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="ID max"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1929,11 +1931,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:R271"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B214" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L225" sqref="L225"/>
+    <sheetView tabSelected="1" topLeftCell="A132" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J147" sqref="J147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11189,7 +11191,7 @@
         <v>225</v>
       </c>
       <c r="B214">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F214">
         <f>ROUND(Taulukko2[[#This Row],[Units 1]]/15,0)+1+Taulukko2[[#This Row],[Is Major 1]]+Taulukko2[[#This Row],[Is in Faction 1]]+Taulukko2[[#This Row],[Is Nato 1]]</f>
@@ -11221,7 +11223,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>1</v>
       </c>
-      <c r="P214" s="3"/>
+      <c r="P214" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="Q214">
         <v>4001</v>
       </c>
@@ -13538,7 +13542,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:Q22"/>
   <sheetViews>
     <sheetView topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">

</xml_diff>

<commit_message>
Finalised officer corps for countries
</commit_message>
<xml_diff>
--- a/Modding resources/Generals rework/Generals_worksheet.xlsx
+++ b/Modding resources/Generals rework/Generals_worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niko\Documents\Paradox Interactive\Hearts of Iron IV\mod\Millennium_Dawn\Modding resources\Generals rework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26FF7493-2110-4AFF-859C-D89A03800DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40DE03DF-8D53-4ED7-A6F5-BF4C0DE92E0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="472">
   <si>
     <t>TAG</t>
   </si>
@@ -1948,8 +1948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:R276"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A205" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P223" sqref="P223"/>
+    <sheetView tabSelected="1" topLeftCell="A193" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P227" sqref="P227"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11556,7 +11556,9 @@
         <f>Taulukko2[[#This Row],[No of FMs 2]]-Taulukko2[[#This Row],[No of FMs 1]]</f>
         <v>-1</v>
       </c>
-      <c r="P223" s="3"/>
+      <c r="P223" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="Q223">
         <v>4101</v>
       </c>
@@ -13683,8 +13685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:Q22"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>